<commit_message>
upload Action plan file , WBS
</commit_message>
<xml_diff>
--- a/AI Project Work Breakdown Structure (WBS).xlsx
+++ b/AI Project Work Breakdown Structure (WBS).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\SIC-AI-KSA-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5ED86C-74EA-4F84-8249-0807355648EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5507C59E-4B53-4BEB-B1A5-EB21F8688518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="819" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,10 +143,6 @@
   </si>
   <si>
     <t>W4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capstone Project Work Breakdown Structure (WBS)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -228,6 +224,45 @@
   </si>
   <si>
     <t>Ruba, Sara, Ghassan, Meshal, Martada, Abdullah</t>
+  </si>
+  <si>
+    <t>Martada , Meshal</t>
+  </si>
+  <si>
+    <t>2. Editing</t>
+  </si>
+  <si>
+    <t>2.1.1  Edit action plan file</t>
+  </si>
+  <si>
+    <t>Capstone Project Work Breakdown Structure (WBS)</t>
+  </si>
+  <si>
+    <t>2.1  Edit Work Breakdown Structuren file</t>
+  </si>
+  <si>
+    <t>Ruba</t>
+  </si>
+  <si>
+    <t>3. Data</t>
+  </si>
+  <si>
+    <t>3.1 Data collection</t>
+  </si>
+  <si>
+    <t>3.1.1 Data analysis</t>
+  </si>
+  <si>
+    <t>4.Model</t>
+  </si>
+  <si>
+    <t>4.1  Model design</t>
+  </si>
+  <si>
+    <t>4.1.1 Model implementation</t>
+  </si>
+  <si>
+    <t>4.1.1.1 Model evaluation</t>
   </si>
 </sst>
 </file>
@@ -803,9 +838,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,6 +867,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,13 +897,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>293914</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>32657</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>587829</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>141515</xdr:rowOff>
@@ -933,13 +968,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1719942</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>97971</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>163287</xdr:rowOff>
@@ -1384,7 +1419,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1402,7 +1437,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1420,7 +1455,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1454,7 +1489,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1568,7 +1603,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1586,7 +1621,7 @@
       <c r="B21" s="3"/>
       <c r="C21" s="44"/>
       <c r="D21" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1604,7 +1639,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="44"/>
       <c r="D22" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1622,7 +1657,7 @@
       <c r="B23" s="3"/>
       <c r="C23" s="44"/>
       <c r="D23" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1656,7 +1691,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1714,314 +1749,324 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AD46"/>
+  <dimension ref="B1:AE46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="13" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="13" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="6.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="27.88671875" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="30" width="6.88671875" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.6640625" style="1"/>
+    <col min="2" max="5" width="6.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="27.88671875" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="31" width="6.88671875" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15" thickBot="1"/>
-    <row r="2" spans="2:30" ht="18" thickBot="1">
+    <row r="1" spans="2:31" ht="15" thickBot="1"/>
+    <row r="2" spans="2:31" ht="18" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="2:30" hidden="1">
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="2:31" hidden="1">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="J3" s="35" t="s">
+      <c r="F3" s="2"/>
+      <c r="K3" s="35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:30" hidden="1">
+    <row r="4" spans="2:31" hidden="1">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="J4" s="35" t="s">
+      <c r="F4" s="2"/>
+      <c r="K4" s="35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:30" hidden="1">
+    <row r="5" spans="2:31" hidden="1">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="J5" s="35" t="s">
+      <c r="F5" s="2"/>
+      <c r="K5" s="35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:30" ht="15" thickBot="1">
-      <c r="J6" s="35"/>
-    </row>
-    <row r="7" spans="2:30" ht="15" thickBot="1">
+    <row r="6" spans="2:31" ht="15" thickBot="1">
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="2:31" ht="15" thickBot="1">
       <c r="B7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="39">
+        <f ca="1">TODAY()</f>
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="8" spans="2:31" ht="15" thickBot="1">
+      <c r="B8" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:31" ht="15" thickBot="1">
+      <c r="B9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="39">
-        <f ca="1">TODAY()</f>
-        <v>45136</v>
-      </c>
-    </row>
-    <row r="8" spans="2:30" ht="15" thickBot="1">
-      <c r="B8" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="2:30" ht="15" thickBot="1">
-      <c r="B9" s="31" t="s">
-        <v>36</v>
-      </c>
       <c r="C9" s="33"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="2:30" ht="15" thickBot="1"/>
-    <row r="11" spans="2:30">
-      <c r="B11" s="47" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="2:31" ht="15" thickBot="1"/>
+    <row r="11" spans="2:31">
+      <c r="B11" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="H11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="54" t="s">
+      <c r="I11" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="51" t="s">
+      <c r="L11" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="54" t="s">
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="53"/>
-      <c r="U11" s="54" t="s">
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="V11" s="52"/>
-      <c r="W11" s="52"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="53"/>
-      <c r="Z11" s="54" t="s">
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="52"/>
+      <c r="AA11" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="AA11" s="52"/>
-      <c r="AB11" s="52"/>
-      <c r="AC11" s="52"/>
-      <c r="AD11" s="55"/>
-    </row>
-    <row r="12" spans="2:30">
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="4" t="s">
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="51"/>
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="54"/>
+    </row>
+    <row r="12" spans="2:31">
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="R12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="S12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="T12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="W12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="X12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="Y12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y12" s="5" t="s">
+      <c r="Z12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Z12" s="5" t="s">
+      <c r="AA12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AA12" s="5" t="s">
+      <c r="AB12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AC12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC12" s="5" t="s">
+      <c r="AD12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AE12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:30">
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="38">
+    <row r="13" spans="2:31">
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="38">
         <v>43466</v>
       </c>
-      <c r="L13" s="36">
+      <c r="M13" s="36">
         <v>43467</v>
       </c>
-      <c r="M13" s="36">
+      <c r="N13" s="36">
         <v>43468</v>
       </c>
-      <c r="N13" s="36">
+      <c r="O13" s="36">
         <v>43469</v>
       </c>
-      <c r="O13" s="36">
+      <c r="P13" s="36">
         <v>43470</v>
       </c>
-      <c r="P13" s="36">
+      <c r="Q13" s="36">
         <v>43471</v>
       </c>
-      <c r="Q13" s="36">
+      <c r="R13" s="36">
         <v>43472</v>
       </c>
-      <c r="R13" s="36">
+      <c r="S13" s="36">
         <v>43473</v>
       </c>
-      <c r="S13" s="36">
+      <c r="T13" s="36">
         <v>43474</v>
       </c>
-      <c r="T13" s="36">
+      <c r="U13" s="36">
         <v>43475</v>
       </c>
-      <c r="U13" s="36">
+      <c r="V13" s="36">
         <v>43476</v>
       </c>
-      <c r="V13" s="36">
+      <c r="W13" s="36">
         <v>43477</v>
       </c>
-      <c r="W13" s="36">
+      <c r="X13" s="36">
         <v>43478</v>
       </c>
-      <c r="X13" s="36">
+      <c r="Y13" s="36">
         <v>43479</v>
       </c>
-      <c r="Y13" s="36">
+      <c r="Z13" s="36">
         <v>43480</v>
       </c>
-      <c r="Z13" s="36">
+      <c r="AA13" s="36">
         <v>43481</v>
       </c>
-      <c r="AA13" s="36">
+      <c r="AB13" s="36">
         <v>43482</v>
       </c>
-      <c r="AB13" s="36">
+      <c r="AC13" s="36">
         <v>43483</v>
       </c>
-      <c r="AC13" s="36">
+      <c r="AD13" s="36">
         <v>43484</v>
       </c>
-      <c r="AD13" s="37">
+      <c r="AE13" s="37">
         <v>43485</v>
       </c>
     </row>
-    <row r="14" spans="2:30" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:31" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10">
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10">
         <f>DATE(2023,7,20)</f>
         <v>45127</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="10">
         <f>DATE(2023,7,25)</f>
         <v>45132</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11" t="s">
+      <c r="I14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
@@ -2033,36 +2078,39 @@
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
       <c r="W14" s="13"/>
-      <c r="X14" s="8"/>
+      <c r="X14" s="13"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
-      <c r="AD14" s="14"/>
-    </row>
-    <row r="15" spans="2:30">
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="14"/>
+    </row>
+    <row r="15" spans="2:31">
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10">
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10">
         <f>DATE(2023,7,20)</f>
         <v>45127</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="10">
         <f>DATE(2023,7,29)</f>
         <v>45136</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11" t="s">
+      <c r="I15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
+      <c r="L15" s="15"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
@@ -2073,41 +2121,47 @@
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
-      <c r="W15" s="8"/>
+      <c r="W15" s="16"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
       <c r="AB15" s="8"/>
       <c r="AC15" s="8"/>
-      <c r="AD15" s="14"/>
-    </row>
-    <row r="16" spans="2:30">
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="14"/>
+    </row>
+    <row r="16" spans="2:31">
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="10">
+      <c r="F16" s="3"/>
+      <c r="G16" s="10">
         <f>DATE(2023,7,29)</f>
         <v>45136</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="18"/>
+      <c r="H16" s="10">
+        <f>DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="17"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
-      <c r="S16" s="8"/>
+      <c r="S16" s="18"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
@@ -2118,31 +2172,40 @@
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="8"/>
-      <c r="AD16" s="14"/>
-    </row>
-    <row r="17" spans="2:30">
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="14"/>
+    </row>
+    <row r="17" spans="2:31">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="18"/>
+      <c r="E17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10">
+        <f>DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" ref="H17" si="0">DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="17"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
-      <c r="S17" s="8"/>
+      <c r="S17" s="18"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -2153,29 +2216,38 @@
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
-      <c r="AD17" s="14"/>
-    </row>
-    <row r="18" spans="2:30">
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="14"/>
+    </row>
+    <row r="18" spans="2:31">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="10">
+        <f>DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="H18" s="10">
+        <f>DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="19"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
-      <c r="Q18" s="8"/>
+      <c r="Q18" s="20"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
@@ -2188,22 +2260,25 @@
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
-      <c r="AD18" s="14"/>
-    </row>
-    <row r="19" spans="2:30">
-      <c r="B19" s="7"/>
+      <c r="AD18" s="8"/>
+      <c r="AE18" s="14"/>
+    </row>
+    <row r="19" spans="2:31">
+      <c r="B19" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -2221,22 +2296,30 @@
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
-      <c r="AD19" s="14"/>
-    </row>
-    <row r="20" spans="2:30">
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="14"/>
+    </row>
+    <row r="20" spans="2:31">
       <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="10">
+        <f>DATE(2023,7,20)</f>
+        <v>45127</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
@@ -2254,22 +2337,33 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
-      <c r="AD20" s="14"/>
-    </row>
-    <row r="21" spans="2:30">
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="14"/>
+    </row>
+    <row r="21" spans="2:31">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10">
+        <f>DATE(2023,7,29)</f>
+        <v>45136</v>
+      </c>
+      <c r="H21" s="10">
+        <f>DATE(2023,7,30)</f>
+        <v>45137</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="7"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
@@ -2287,22 +2381,25 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
-      <c r="AD21" s="14"/>
-    </row>
-    <row r="22" spans="2:30">
-      <c r="B22" s="7"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="14"/>
+    </row>
+    <row r="22" spans="2:31">
+      <c r="B22" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
+      <c r="L22" s="7"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -2320,22 +2417,31 @@
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
-      <c r="AD22" s="14"/>
-    </row>
-    <row r="23" spans="2:30" ht="17.100000000000001" customHeight="1">
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="14"/>
+    </row>
+    <row r="23" spans="2:31" ht="17.100000000000001" customHeight="1">
       <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11" t="s">
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10">
+        <f>DATE(2023,8,1)</f>
+        <v>45139</v>
+      </c>
+      <c r="H23" s="10">
+        <f>DATE(2023,8,3)</f>
+        <v>45141</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
+      <c r="L23" s="7"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -2353,22 +2459,31 @@
       <c r="AA23" s="8"/>
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
-      <c r="AD23" s="14"/>
-    </row>
-    <row r="24" spans="2:30">
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="14"/>
+    </row>
+    <row r="24" spans="2:31">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11" t="s">
+      <c r="D24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10">
+        <f>DATE(2023,8,5)</f>
+        <v>45143</v>
+      </c>
+      <c r="H24" s="10">
+        <f>DATE(2023,8,6)</f>
+        <v>45144</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
+      <c r="L24" s="7"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -2386,22 +2501,25 @@
       <c r="AA24" s="8"/>
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
-      <c r="AD24" s="14"/>
-    </row>
-    <row r="25" spans="2:30">
-      <c r="B25" s="7"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="14"/>
+    </row>
+    <row r="25" spans="2:31">
+      <c r="B25" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="11" t="s">
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
+      <c r="L25" s="7"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -2419,22 +2537,25 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AD25" s="14"/>
-    </row>
-    <row r="26" spans="2:30">
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="14"/>
+    </row>
+    <row r="26" spans="2:31">
       <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="11" t="s">
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="7"/>
-      <c r="L26" s="8"/>
+      <c r="L26" s="7"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
@@ -2452,22 +2573,25 @@
       <c r="AA26" s="8"/>
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
-      <c r="AD26" s="14"/>
-    </row>
-    <row r="27" spans="2:30">
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="14"/>
+    </row>
+    <row r="27" spans="2:31">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
+      <c r="D27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="11" t="s">
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
+      <c r="L27" s="7"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
@@ -2485,22 +2609,25 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
-      <c r="AD27" s="14"/>
-    </row>
-    <row r="28" spans="2:30">
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="14"/>
+    </row>
+    <row r="28" spans="2:31">
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
+      <c r="E28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="9"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="11" t="s">
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
+      <c r="L28" s="7"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
@@ -2518,22 +2645,23 @@
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
-      <c r="AD28" s="14"/>
-    </row>
-    <row r="29" spans="2:30">
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="14"/>
+    </row>
+    <row r="29" spans="2:31">
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11" t="s">
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="7"/>
-      <c r="L29" s="8"/>
+      <c r="L29" s="7"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8"/>
@@ -2551,22 +2679,23 @@
       <c r="AA29" s="8"/>
       <c r="AB29" s="8"/>
       <c r="AC29" s="8"/>
-      <c r="AD29" s="14"/>
-    </row>
-    <row r="30" spans="2:30">
+      <c r="AD29" s="8"/>
+      <c r="AE29" s="14"/>
+    </row>
+    <row r="30" spans="2:31">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="11" t="s">
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="8"/>
+      <c r="L30" s="7"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
@@ -2584,20 +2713,21 @@
       <c r="AA30" s="8"/>
       <c r="AB30" s="8"/>
       <c r="AC30" s="8"/>
-      <c r="AD30" s="14"/>
-    </row>
-    <row r="31" spans="2:30" ht="17.100000000000001" customHeight="1">
+      <c r="AD30" s="8"/>
+      <c r="AE30" s="14"/>
+    </row>
+    <row r="31" spans="2:31" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="21"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="8"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="7"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
@@ -2615,20 +2745,21 @@
       <c r="AA31" s="8"/>
       <c r="AB31" s="8"/>
       <c r="AC31" s="8"/>
-      <c r="AD31" s="14"/>
-    </row>
-    <row r="32" spans="2:30">
+      <c r="AD31" s="8"/>
+      <c r="AE31" s="14"/>
+    </row>
+    <row r="32" spans="2:31">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="21"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="8"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
@@ -2646,20 +2777,21 @@
       <c r="AA32" s="8"/>
       <c r="AB32" s="8"/>
       <c r="AC32" s="8"/>
-      <c r="AD32" s="14"/>
-    </row>
-    <row r="33" spans="2:30">
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="14"/>
+    </row>
+    <row r="33" spans="2:31">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="21"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="8"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="7"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
@@ -2677,20 +2809,21 @@
       <c r="AA33" s="8"/>
       <c r="AB33" s="8"/>
       <c r="AC33" s="8"/>
-      <c r="AD33" s="14"/>
-    </row>
-    <row r="34" spans="2:30">
+      <c r="AD33" s="8"/>
+      <c r="AE33" s="14"/>
+    </row>
+    <row r="34" spans="2:31">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="21"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="8"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="7"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
@@ -2708,20 +2841,21 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
       <c r="AC34" s="8"/>
-      <c r="AD34" s="14"/>
-    </row>
-    <row r="35" spans="2:30">
+      <c r="AD34" s="8"/>
+      <c r="AE34" s="14"/>
+    </row>
+    <row r="35" spans="2:31">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="8"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="7"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -2739,20 +2873,21 @@
       <c r="AA35" s="8"/>
       <c r="AB35" s="8"/>
       <c r="AC35" s="8"/>
-      <c r="AD35" s="14"/>
-    </row>
-    <row r="36" spans="2:30">
+      <c r="AD35" s="8"/>
+      <c r="AE35" s="14"/>
+    </row>
+    <row r="36" spans="2:31">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="21"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="8"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="7"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
@@ -2770,20 +2905,21 @@
       <c r="AA36" s="8"/>
       <c r="AB36" s="8"/>
       <c r="AC36" s="8"/>
-      <c r="AD36" s="14"/>
-    </row>
-    <row r="37" spans="2:30">
+      <c r="AD36" s="8"/>
+      <c r="AE36" s="14"/>
+    </row>
+    <row r="37" spans="2:31">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="8"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="7"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
@@ -2801,20 +2937,21 @@
       <c r="AA37" s="8"/>
       <c r="AB37" s="8"/>
       <c r="AC37" s="8"/>
-      <c r="AD37" s="14"/>
-    </row>
-    <row r="38" spans="2:30">
+      <c r="AD37" s="8"/>
+      <c r="AE37" s="14"/>
+    </row>
+    <row r="38" spans="2:31">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="21"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="21"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="8"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
@@ -2832,20 +2969,21 @@
       <c r="AA38" s="8"/>
       <c r="AB38" s="8"/>
       <c r="AC38" s="8"/>
-      <c r="AD38" s="14"/>
-    </row>
-    <row r="39" spans="2:30" ht="17.100000000000001" customHeight="1">
+      <c r="AD38" s="8"/>
+      <c r="AE38" s="14"/>
+    </row>
+    <row r="39" spans="2:31" ht="17.100000000000001" customHeight="1">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="21"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="8"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="7"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
@@ -2863,20 +3001,21 @@
       <c r="AA39" s="8"/>
       <c r="AB39" s="8"/>
       <c r="AC39" s="8"/>
-      <c r="AD39" s="14"/>
-    </row>
-    <row r="40" spans="2:30">
+      <c r="AD39" s="8"/>
+      <c r="AE39" s="14"/>
+    </row>
+    <row r="40" spans="2:31">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="21"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="8"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="7"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -2894,20 +3033,21 @@
       <c r="AA40" s="8"/>
       <c r="AB40" s="8"/>
       <c r="AC40" s="8"/>
-      <c r="AD40" s="14"/>
-    </row>
-    <row r="41" spans="2:30">
+      <c r="AD40" s="8"/>
+      <c r="AE40" s="14"/>
+    </row>
+    <row r="41" spans="2:31">
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="21"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="8"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="7"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
@@ -2925,20 +3065,21 @@
       <c r="AA41" s="8"/>
       <c r="AB41" s="8"/>
       <c r="AC41" s="8"/>
-      <c r="AD41" s="14"/>
-    </row>
-    <row r="42" spans="2:30">
+      <c r="AD41" s="8"/>
+      <c r="AE41" s="14"/>
+    </row>
+    <row r="42" spans="2:31">
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="21"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="21"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="8"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="7"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
@@ -2956,20 +3097,21 @@
       <c r="AA42" s="8"/>
       <c r="AB42" s="8"/>
       <c r="AC42" s="8"/>
-      <c r="AD42" s="14"/>
-    </row>
-    <row r="43" spans="2:30">
+      <c r="AD42" s="8"/>
+      <c r="AE42" s="14"/>
+    </row>
+    <row r="43" spans="2:31">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="21"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="8"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="7"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -2987,20 +3129,21 @@
       <c r="AA43" s="8"/>
       <c r="AB43" s="8"/>
       <c r="AC43" s="8"/>
-      <c r="AD43" s="14"/>
-    </row>
-    <row r="44" spans="2:30">
+      <c r="AD43" s="8"/>
+      <c r="AE43" s="14"/>
+    </row>
+    <row r="44" spans="2:31">
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="21"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="21"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="8"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="7"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
@@ -3018,20 +3161,21 @@
       <c r="AA44" s="8"/>
       <c r="AB44" s="8"/>
       <c r="AC44" s="8"/>
-      <c r="AD44" s="14"/>
-    </row>
-    <row r="45" spans="2:30">
+      <c r="AD44" s="8"/>
+      <c r="AE44" s="14"/>
+    </row>
+    <row r="45" spans="2:31">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="21"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="8"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="7"/>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
@@ -3049,20 +3193,21 @@
       <c r="AA45" s="8"/>
       <c r="AB45" s="8"/>
       <c r="AC45" s="8"/>
-      <c r="AD45" s="14"/>
-    </row>
-    <row r="46" spans="2:30" ht="15" thickBot="1">
+      <c r="AD45" s="8"/>
+      <c r="AE45" s="14"/>
+    </row>
+    <row r="46" spans="2:31" ht="15" thickBot="1">
       <c r="B46" s="22"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="25"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="24"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="23"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="22"/>
       <c r="M46" s="23"/>
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
@@ -3080,25 +3225,26 @@
       <c r="AA46" s="23"/>
       <c r="AB46" s="23"/>
       <c r="AC46" s="23"/>
-      <c r="AD46" s="27"/>
+      <c r="AD46" s="23"/>
+      <c r="AE46" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B11:E13"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="P11:T11"/>
-    <mergeCell ref="U11:Y11"/>
-    <mergeCell ref="Z11:AD11"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="B11:F13"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:U11"/>
+    <mergeCell ref="V11:Z11"/>
+    <mergeCell ref="AA11:AE11"/>
     <mergeCell ref="G11:G13"/>
+    <mergeCell ref="K11:K13"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J46" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>$J$3:$J$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K14:K46" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>$K$3:$K$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>